<commit_message>
Fixed error in Brazils 2017 week 4 epi data (got mistaken with week 4 2016) and imputed using quadratic instead of linear interpolation
</commit_message>
<xml_diff>
--- a/data/Brazil/excel_files/Cases2017.xlsx
+++ b/data/Brazil/excel_files/Cases2017.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\ziknet-trends-backend\data\Brazil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\ziknet-trends-backend\data\Brazil\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9544D376-C5E3-4854-A780-47FCD95F7654}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D510F158-C562-4B91-8393-31313A7F90F5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{D1220306-A291-47C7-A248-7ECD7104F77E}"/>
   </bookViews>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C234F185-508A-41E2-A998-D9731E709D71}">
   <dimension ref="A1:DA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="AW34" sqref="AW34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +854,7 @@
       </c>
       <c r="E2" s="2">
         <f>SUM(E3:E9)</f>
-        <v>973</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
@@ -1330,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -1398,7 +1398,7 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>443</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <v>100</v>
@@ -1466,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>383</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>94</v>
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>27</v>
@@ -1602,7 +1602,7 @@
         <v>6</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>91</v>
@@ -1670,7 +1670,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="H9">
         <v>186</v>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="3"/>
-        <v>6217</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="3"/>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="CE10" s="2">
-        <f t="shared" ref="CE10:EE10" si="5">SUM(CE11:CE19)</f>
+        <f t="shared" ref="CE10:DA10" si="5">SUM(CE11:CE19)</f>
         <v>0</v>
       </c>
       <c r="CF10" s="2">
@@ -2159,7 +2159,7 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <v>11</v>
@@ -2227,7 +2227,7 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <v>5687</v>
+        <v>58</v>
       </c>
       <c r="H12">
         <v>325</v>
@@ -2295,7 +2295,7 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <v>91</v>
@@ -2363,7 +2363,7 @@
         <v>12</v>
       </c>
       <c r="E14">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>56</v>
@@ -2431,7 +2431,7 @@
         <v>13</v>
       </c>
       <c r="E15">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -2499,7 +2499,7 @@
         <v>14</v>
       </c>
       <c r="E16">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>4</v>
@@ -2567,7 +2567,7 @@
         <v>15</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2635,7 +2635,7 @@
         <v>16</v>
       </c>
       <c r="E18">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="H18">
         <v>21</v>
@@ -2703,7 +2703,7 @@
         <v>17</v>
       </c>
       <c r="E19">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>7</v>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="E20" s="2">
         <f t="shared" si="6"/>
-        <v>15653</v>
+        <v>86</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="6"/>
@@ -3095,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="CE20" s="2">
-        <f t="shared" ref="CE20:EE20" si="8">SUM(CE21:CE24)</f>
+        <f t="shared" ref="CE20:DA20" si="8">SUM(CE21:CE24)</f>
         <v>0</v>
       </c>
       <c r="CF20" s="2">
@@ -3192,7 +3192,7 @@
         <v>19</v>
       </c>
       <c r="E21">
-        <v>557</v>
+        <v>16</v>
       </c>
       <c r="H21">
         <v>41</v>
@@ -3260,7 +3260,7 @@
         <v>20</v>
       </c>
       <c r="E22">
-        <v>702</v>
+        <v>45</v>
       </c>
       <c r="H22">
         <v>122</v>
@@ -3328,7 +3328,7 @@
         <v>21</v>
       </c>
       <c r="E23">
-        <v>14081</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3396,7 +3396,7 @@
         <v>22</v>
       </c>
       <c r="E24">
-        <v>313</v>
+        <v>24</v>
       </c>
       <c r="H24">
         <v>114</v>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="E25" s="2">
         <f t="shared" si="9"/>
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="9"/>
@@ -3788,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="CE25" s="2">
-        <f t="shared" ref="CE25:EE25" si="11">SUM(CE26:CE28)</f>
+        <f t="shared" ref="CE25:DA25" si="11">SUM(CE26:CE28)</f>
         <v>0</v>
       </c>
       <c r="CF25" s="2">
@@ -3885,7 +3885,7 @@
         <v>24</v>
       </c>
       <c r="E26">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="H26">
         <v>37</v>
@@ -3953,7 +3953,7 @@
         <v>25</v>
       </c>
       <c r="E27">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H27">
         <v>22</v>
@@ -4021,7 +4021,7 @@
         <v>26</v>
       </c>
       <c r="E28">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H28">
         <v>12</v>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="E29" s="2">
         <f t="shared" si="12"/>
-        <v>7731</v>
+        <v>50</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="12"/>
@@ -4510,7 +4510,7 @@
         <v>28</v>
       </c>
       <c r="E30">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="H30">
         <v>19</v>
@@ -4578,7 +4578,7 @@
         <v>29</v>
       </c>
       <c r="E31">
-        <v>217</v>
+        <v>45</v>
       </c>
       <c r="H31">
         <v>213</v>
@@ -4646,7 +4646,7 @@
         <v>30</v>
       </c>
       <c r="E32">
-        <v>7150</v>
+        <v>2</v>
       </c>
       <c r="H32">
         <v>27</v>
@@ -4714,7 +4714,7 @@
         <v>31</v>
       </c>
       <c r="E33">
-        <v>339</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>7</v>
@@ -4795,7 +4795,7 @@
       </c>
       <c r="E34" s="2">
         <f>SUM(E3:E9)+SUM(E11:E19)+SUM(E21:E24)+SUM(E26:E28)+SUM(E30:E33)</f>
-        <v>30683</v>
+        <v>316</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="16"/>
@@ -5150,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="CP34" s="2">
-        <f t="shared" ref="CP34:EP34" si="20">SUM(CP3:CP9)+SUM(CP11:CP19)+SUM(CP21:CP24)+SUM(CP26:CP28)+SUM(CP30:CP33)</f>
+        <f t="shared" ref="CP34:DA34" si="20">SUM(CP3:CP9)+SUM(CP11:CP19)+SUM(CP21:CP24)+SUM(CP26:CP28)+SUM(CP30:CP33)</f>
         <v>0</v>
       </c>
       <c r="CQ34" s="2">

</xml_diff>